<commit_message>
Maint: update test output
</commit_message>
<xml_diff>
--- a/tests/Overall/Composicoes/composicoes_composition_teste.xlsx
+++ b/tests/Overall/Composicoes/composicoes_composition_teste.xlsx
@@ -677,16 +677,16 @@
         <v>35</v>
       </c>
       <c r="C3">
-        <v>101.325</v>
+        <v>9936.588112500001</v>
       </c>
       <c r="D3">
-        <v>318.4952793422599</v>
+        <v>134907.7581017592</v>
       </c>
       <c r="E3">
-        <v>8296.190515929531</v>
+        <v>3514088.075655271</v>
       </c>
       <c r="F3">
-        <v>1.312672665700222</v>
+        <v>1.590786763863847</v>
       </c>
       <c r="G3">
         <v>26.04808</v>
@@ -701,7 +701,7 @@
         <v>173.0671113309112</v>
       </c>
       <c r="K3">
-        <v>4200.383205412815</v>
+        <v>3025.885112537143</v>
       </c>
       <c r="L3">
         <v>4200.16193522986</v>
@@ -710,19 +710,19 @@
         <v>0.6636106088685741</v>
       </c>
       <c r="N3">
-        <v>1.326783294303116</v>
+        <v>774.839307540194</v>
       </c>
       <c r="O3">
         <v>1.386509054431758</v>
       </c>
       <c r="P3">
-        <v>33.29874407248995</v>
+        <v>33.36810169136437</v>
       </c>
       <c r="Q3">
         <v>33.64915788153957</v>
       </c>
       <c r="R3">
-        <v>0.9925954477440434</v>
+        <v>0.1670631120265793</v>
       </c>
       <c r="S3">
         <v>0.9920264880486523</v>
@@ -731,7 +731,7 @@
         <v>163.8318774589159</v>
       </c>
       <c r="U3">
-        <v>2.741794420180521</v>
+        <v>1177.239333887838</v>
       </c>
       <c r="V3">
         <v>2.96306465605617</v>
@@ -743,7 +743,7 @@
         <v>18.01852792136123</v>
       </c>
       <c r="Y3">
-        <v>18.01867468422456</v>
+        <v>18.09164673579438</v>
       </c>
       <c r="Z3">
         <v>-1</v>

</xml_diff>

<commit_message>
Update: use new version of DWSIM
</commit_message>
<xml_diff>
--- a/tests/Overall/Composicoes/composicoes_composition_teste.xlsx
+++ b/tests/Overall/Composicoes/composicoes_composition_teste.xlsx
@@ -698,49 +698,49 @@
         <v>-1</v>
       </c>
       <c r="J3">
-        <v>173.0671113309112</v>
+        <v>173.0671113313479</v>
       </c>
       <c r="K3">
         <v>3025.885112537143</v>
       </c>
       <c r="L3">
-        <v>4200.16193522986</v>
+        <v>4200.16193524045</v>
       </c>
       <c r="M3">
-        <v>0.6636106088685741</v>
+        <v>0.6636106088905102</v>
       </c>
       <c r="N3">
         <v>774.839307540194</v>
       </c>
       <c r="O3">
-        <v>1.386509054431758</v>
+        <v>1.386509054431434</v>
       </c>
       <c r="P3">
         <v>33.36810169136437</v>
       </c>
       <c r="Q3">
-        <v>33.64915788153957</v>
+        <v>33.64915788153163</v>
       </c>
       <c r="R3">
         <v>0.1670631120265793</v>
       </c>
       <c r="S3">
-        <v>0.9920264880486523</v>
+        <v>0.9920264880486497</v>
       </c>
       <c r="T3">
-        <v>163.8318774589159</v>
+        <v>163.8318774564127</v>
       </c>
       <c r="U3">
         <v>1177.239333887838</v>
       </c>
       <c r="V3">
-        <v>2.96306465605617</v>
+        <v>2.963064656010855</v>
       </c>
       <c r="W3">
-        <v>0.3363893911042831</v>
+        <v>0.3363893911094898</v>
       </c>
       <c r="X3">
-        <v>18.01852792136123</v>
+        <v>18.01852792136104</v>
       </c>
       <c r="Y3">
         <v>18.09164673579438</v>

</xml_diff>